<commit_message>
Nova versão do relatorio
</commit_message>
<xml_diff>
--- a/graficos.xlsx
+++ b/graficos.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Miguel\OneDrive\Faculdade\2º Ano\2º Semestre\ASA\Projetos\ASA-P1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jovma\Documents\ASA-P1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{3572D594-0744-4263-AA76-945BC4350AB8}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{25DC4B96-69F5-4624-88E3-909923F701B4}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD7A30B1-1C6A-4DF4-B17D-037501C70C62}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7965" xr2:uid="{BFF67A87-D1DC-4EF5-8268-33A2630A7605}"/>
   </bookViews>
@@ -57,7 +57,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="28">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -408,11 +408,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
@@ -428,13 +446,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
@@ -446,9 +461,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -456,6 +468,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
@@ -470,10 +491,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -493,8 +518,2033 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Folha1!$B$3:$B$52</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>15000</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>150000</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>90000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Folha1!$D$3:$D$52</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>1E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.0000000000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2.4999999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.31719999999999998</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.18209999999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D570-46B1-817B-F57CC7BB7949}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="356220376"/>
+        <c:axId val="356214144"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="356220376"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Vértices</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> + Arestas</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="356214144"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="356214144"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Tempo de execução (ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="356220376"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Folha1!$B$3:$B$52</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>15000</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>150000</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>90000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Folha1!$F$3:$F$52</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>8696</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>40000</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>343120</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>3466880</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>2047968</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-68D9-4872-9C85-93E6F2499FE9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="594575512"/>
+        <c:axId val="594576824"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="594575512"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Vértices</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> + Arestas</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="594576824"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="594576824"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Memória ocupada (bytes)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="594575512"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>300036</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>104774</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>400049</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>47624</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F212D95C-D2F1-4AAE-81F0-8F36D8134946}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>376237</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>47624</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>47624</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{02A5ACBC-23C5-4AFA-B9FC-D0B7703A9A03}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -790,10 +2840,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F895D286-5180-403D-925E-F08247EAC5D6}">
-  <dimension ref="B1:F42"/>
+  <dimension ref="B1:Y62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView tabSelected="1" topLeftCell="D29" workbookViewId="0">
+      <selection activeCell="Y42" sqref="Y42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -806,396 +2856,556 @@
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="26"/>
-      <c r="E2" s="27" t="s">
+      <c r="D2" s="27"/>
+      <c r="E2" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="28"/>
+      <c r="F2" s="14"/>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="20">
+      <c r="B3" s="18">
         <v>150</v>
       </c>
       <c r="C3" s="4">
         <v>1E-3</v>
       </c>
-      <c r="D3" s="16">
+      <c r="D3" s="15">
         <v>1E-3</v>
       </c>
       <c r="E3" s="7"/>
-      <c r="F3" s="16"/>
+      <c r="F3" s="15">
+        <v>8696</v>
+      </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="21"/>
+      <c r="B4" s="19"/>
       <c r="C4" s="5">
         <v>1E-3</v>
       </c>
-      <c r="D4" s="17"/>
+      <c r="D4" s="16"/>
       <c r="E4" s="3"/>
-      <c r="F4" s="17"/>
+      <c r="F4" s="16"/>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="21"/>
+      <c r="B5" s="19"/>
       <c r="C5" s="5">
         <v>1E-3</v>
       </c>
-      <c r="D5" s="17"/>
+      <c r="D5" s="16"/>
       <c r="E5" s="3"/>
-      <c r="F5" s="17"/>
+      <c r="F5" s="16"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="21"/>
+      <c r="B6" s="19"/>
       <c r="C6" s="5">
         <v>1E-3</v>
       </c>
-      <c r="D6" s="17"/>
+      <c r="D6" s="16"/>
       <c r="E6" s="3"/>
-      <c r="F6" s="17"/>
+      <c r="F6" s="16"/>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="21"/>
+      <c r="B7" s="19"/>
       <c r="C7" s="5">
         <v>1E-3</v>
       </c>
-      <c r="D7" s="17"/>
+      <c r="D7" s="16"/>
       <c r="E7" s="3"/>
-      <c r="F7" s="17"/>
+      <c r="F7" s="16"/>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="21"/>
+      <c r="B8" s="19"/>
       <c r="C8" s="5">
         <v>1E-3</v>
       </c>
-      <c r="D8" s="17"/>
+      <c r="D8" s="16"/>
       <c r="E8" s="3"/>
-      <c r="F8" s="17"/>
+      <c r="F8" s="16"/>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="21"/>
+      <c r="B9" s="19"/>
       <c r="C9" s="5">
         <v>1E-3</v>
       </c>
-      <c r="D9" s="17"/>
+      <c r="D9" s="16"/>
       <c r="E9" s="3"/>
-      <c r="F9" s="17"/>
+      <c r="F9" s="16"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="21"/>
+      <c r="B10" s="19"/>
       <c r="C10" s="5">
         <v>1E-3</v>
       </c>
-      <c r="D10" s="17"/>
+      <c r="D10" s="16"/>
       <c r="E10" s="3"/>
-      <c r="F10" s="17"/>
+      <c r="F10" s="16"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="21"/>
+      <c r="B11" s="19"/>
       <c r="C11" s="5">
         <v>1E-3</v>
       </c>
-      <c r="D11" s="17"/>
+      <c r="D11" s="16"/>
       <c r="E11" s="3"/>
-      <c r="F11" s="17"/>
+      <c r="F11" s="16"/>
     </row>
     <row r="12" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="22"/>
+      <c r="B12" s="20"/>
       <c r="C12" s="6">
         <v>1E-3</v>
       </c>
-      <c r="D12" s="18"/>
+      <c r="D12" s="17"/>
       <c r="E12" s="8"/>
-      <c r="F12" s="18"/>
+      <c r="F12" s="17"/>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="13">
+      <c r="B13" s="21">
         <v>1500</v>
       </c>
       <c r="C13" s="10">
         <v>1E-3</v>
       </c>
-      <c r="D13" s="23">
+      <c r="D13" s="24">
         <f>AVERAGE(C13:C22)</f>
-        <v>1.1000000000000003E-3</v>
+        <v>1.0000000000000002E-3</v>
       </c>
       <c r="E13" s="7"/>
-      <c r="F13" s="16"/>
+      <c r="F13" s="15">
+        <v>40000</v>
+      </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="14"/>
+      <c r="B14" s="22"/>
       <c r="C14" s="3">
         <v>1E-3</v>
       </c>
-      <c r="D14" s="24"/>
+      <c r="D14" s="25"/>
       <c r="E14" s="3"/>
-      <c r="F14" s="17"/>
+      <c r="F14" s="16"/>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="14"/>
+      <c r="B15" s="22"/>
       <c r="C15" s="2">
-        <v>2E-3</v>
-      </c>
-      <c r="D15" s="24"/>
+        <v>1E-3</v>
+      </c>
+      <c r="D15" s="25"/>
       <c r="E15" s="3"/>
-      <c r="F15" s="17"/>
+      <c r="F15" s="16"/>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B16" s="14"/>
+      <c r="B16" s="22"/>
       <c r="C16" s="3">
         <v>1E-3</v>
       </c>
-      <c r="D16" s="24"/>
+      <c r="D16" s="25"/>
       <c r="E16" s="3"/>
-      <c r="F16" s="17"/>
+      <c r="F16" s="16"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="14"/>
+      <c r="B17" s="22"/>
       <c r="C17" s="3">
         <v>1E-3</v>
       </c>
-      <c r="D17" s="24"/>
+      <c r="D17" s="25"/>
       <c r="E17" s="3"/>
-      <c r="F17" s="17"/>
+      <c r="F17" s="16"/>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="14"/>
+      <c r="B18" s="22"/>
       <c r="C18" s="3">
         <v>1E-3</v>
       </c>
-      <c r="D18" s="24"/>
+      <c r="D18" s="25"/>
       <c r="E18" s="3"/>
-      <c r="F18" s="17"/>
+      <c r="F18" s="16"/>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="14"/>
+      <c r="B19" s="22"/>
       <c r="C19" s="3">
         <v>1E-3</v>
       </c>
-      <c r="D19" s="24"/>
+      <c r="D19" s="25"/>
       <c r="E19" s="3"/>
-      <c r="F19" s="17"/>
+      <c r="F19" s="16"/>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="14"/>
+      <c r="B20" s="22"/>
       <c r="C20" s="3">
         <v>1E-3</v>
       </c>
-      <c r="D20" s="24"/>
+      <c r="D20" s="25"/>
       <c r="E20" s="3"/>
-      <c r="F20" s="17"/>
+      <c r="F20" s="16"/>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B21" s="14"/>
+      <c r="B21" s="22"/>
       <c r="C21" s="3">
         <v>1E-3</v>
       </c>
-      <c r="D21" s="24"/>
+      <c r="D21" s="25"/>
       <c r="E21" s="3"/>
-      <c r="F21" s="17"/>
+      <c r="F21" s="16"/>
     </row>
     <row r="22" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="15"/>
+      <c r="B22" s="23"/>
       <c r="C22" s="8">
         <v>1E-3</v>
       </c>
-      <c r="D22" s="25"/>
+      <c r="D22" s="26"/>
       <c r="E22" s="8"/>
-      <c r="F22" s="18"/>
+      <c r="F22" s="17"/>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="13">
+      <c r="B23" s="21">
         <v>15000</v>
       </c>
       <c r="C23" s="4">
-        <v>9.1999999999999998E-2</v>
-      </c>
-      <c r="D23" s="16">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="D23" s="15">
         <f>AVERAGE(C23:C32)</f>
-        <v>0.1091</v>
+        <v>2.4999999999999998E-2</v>
       </c>
       <c r="E23" s="7"/>
-      <c r="F23" s="16"/>
+      <c r="F23" s="15">
+        <v>343120</v>
+      </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="14"/>
+      <c r="B24" s="22"/>
       <c r="C24" s="5">
-        <v>0.105</v>
-      </c>
-      <c r="D24" s="17"/>
+        <v>1.9E-2</v>
+      </c>
+      <c r="D24" s="16"/>
       <c r="E24" s="3"/>
-      <c r="F24" s="17"/>
+      <c r="F24" s="16"/>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B25" s="14"/>
+      <c r="B25" s="22"/>
       <c r="C25" s="5">
-        <v>0.113</v>
-      </c>
-      <c r="D25" s="17"/>
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="D25" s="16"/>
       <c r="E25" s="3"/>
-      <c r="F25" s="17"/>
+      <c r="F25" s="16"/>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B26" s="14"/>
+      <c r="B26" s="22"/>
       <c r="C26" s="5">
-        <v>0.11</v>
-      </c>
-      <c r="D26" s="17"/>
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="D26" s="16"/>
       <c r="E26" s="3"/>
-      <c r="F26" s="17"/>
+      <c r="F26" s="16"/>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B27" s="14"/>
+      <c r="B27" s="22"/>
       <c r="C27" s="5">
-        <v>0.12</v>
-      </c>
-      <c r="D27" s="17"/>
+        <v>2.3E-2</v>
+      </c>
+      <c r="D27" s="16"/>
       <c r="E27" s="3"/>
-      <c r="F27" s="17"/>
+      <c r="F27" s="16"/>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B28" s="14"/>
+      <c r="B28" s="22"/>
       <c r="C28" s="5">
-        <v>0.112</v>
-      </c>
-      <c r="D28" s="17"/>
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="D28" s="16"/>
       <c r="E28" s="3"/>
-      <c r="F28" s="17"/>
+      <c r="F28" s="16"/>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B29" s="14"/>
+      <c r="B29" s="22"/>
       <c r="C29" s="5">
-        <v>0.109</v>
-      </c>
-      <c r="D29" s="17"/>
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="D29" s="16"/>
       <c r="E29" s="3"/>
-      <c r="F29" s="17"/>
+      <c r="F29" s="16"/>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B30" s="14"/>
+      <c r="B30" s="22"/>
       <c r="C30" s="5">
-        <v>8.7999999999999995E-2</v>
-      </c>
-      <c r="D30" s="17"/>
+        <v>0.02</v>
+      </c>
+      <c r="D30" s="16"/>
       <c r="E30" s="3"/>
-      <c r="F30" s="17"/>
+      <c r="F30" s="16"/>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B31" s="14"/>
+      <c r="B31" s="22"/>
       <c r="C31" s="5">
-        <v>0.12</v>
-      </c>
-      <c r="D31" s="17"/>
+        <v>2.7E-2</v>
+      </c>
+      <c r="D31" s="16"/>
       <c r="E31" s="3"/>
-      <c r="F31" s="17"/>
+      <c r="F31" s="16"/>
     </row>
     <row r="32" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="15"/>
+      <c r="B32" s="23"/>
       <c r="C32" s="6">
-        <v>0.122</v>
-      </c>
-      <c r="D32" s="18"/>
+        <v>0.03</v>
+      </c>
+      <c r="D32" s="17"/>
       <c r="E32" s="8"/>
-      <c r="F32" s="18"/>
-    </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B33" s="13">
+      <c r="F32" s="17"/>
+    </row>
+    <row r="33" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B33" s="21">
         <v>150000</v>
       </c>
       <c r="C33" s="7">
-        <v>0.16700000000000001</v>
-      </c>
-      <c r="D33" s="16">
+        <v>0.311</v>
+      </c>
+      <c r="D33" s="15">
         <f>AVERAGE(C33:C42)</f>
-        <v>0.17339999999999997</v>
+        <v>0.31719999999999998</v>
       </c>
       <c r="E33" s="4"/>
-      <c r="F33" s="16"/>
-    </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B34" s="14"/>
+      <c r="F33" s="15">
+        <v>3466880</v>
+      </c>
+    </row>
+    <row r="34" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B34" s="22"/>
       <c r="C34" s="3">
-        <v>0.17599999999999999</v>
-      </c>
-      <c r="D34" s="17"/>
+        <v>0.32600000000000001</v>
+      </c>
+      <c r="D34" s="16"/>
       <c r="E34" s="5"/>
-      <c r="F34" s="17"/>
-    </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B35" s="14"/>
+      <c r="F34" s="16"/>
+    </row>
+    <row r="35" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B35" s="22"/>
       <c r="C35" s="3">
+        <v>0.315</v>
+      </c>
+      <c r="D35" s="16"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="16"/>
+    </row>
+    <row r="36" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B36" s="22"/>
+      <c r="C36" s="3">
+        <v>0.315</v>
+      </c>
+      <c r="D36" s="16"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="16"/>
+    </row>
+    <row r="37" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B37" s="22"/>
+      <c r="C37" s="3">
+        <v>0.32100000000000001</v>
+      </c>
+      <c r="D37" s="16"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="16"/>
+    </row>
+    <row r="38" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B38" s="22"/>
+      <c r="C38" s="3">
+        <v>0.312</v>
+      </c>
+      <c r="D38" s="16"/>
+      <c r="E38" s="5"/>
+      <c r="F38" s="16"/>
+    </row>
+    <row r="39" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B39" s="22"/>
+      <c r="C39" s="3">
+        <v>0.32400000000000001</v>
+      </c>
+      <c r="D39" s="16"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="16"/>
+    </row>
+    <row r="40" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B40" s="22"/>
+      <c r="C40" s="9">
+        <v>0.311</v>
+      </c>
+      <c r="D40" s="16"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="16"/>
+    </row>
+    <row r="41" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B41" s="22"/>
+      <c r="C41" s="12">
+        <v>0.308</v>
+      </c>
+      <c r="D41" s="28"/>
+      <c r="E41" s="5"/>
+      <c r="F41" s="16"/>
+    </row>
+    <row r="42" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B42" s="23"/>
+      <c r="C42" s="11">
+        <v>0.32900000000000001</v>
+      </c>
+      <c r="D42" s="17"/>
+      <c r="E42" s="6"/>
+      <c r="F42" s="17"/>
+      <c r="Y42">
+        <f ca="1">Y42</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B43" s="31">
+        <v>90000</v>
+      </c>
+      <c r="C43" s="30">
         <v>0.17399999999999999</v>
       </c>
-      <c r="D35" s="17"/>
-      <c r="E35" s="5"/>
-      <c r="F35" s="17"/>
-    </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B36" s="14"/>
-      <c r="C36" s="3">
-        <v>0.17199999999999999</v>
-      </c>
-      <c r="D36" s="17"/>
-      <c r="E36" s="5"/>
-      <c r="F36" s="17"/>
-    </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B37" s="14"/>
-      <c r="C37" s="3">
-        <v>0.16500000000000001</v>
-      </c>
-      <c r="D37" s="17"/>
-      <c r="E37" s="5"/>
-      <c r="F37" s="17"/>
-    </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B38" s="14"/>
-      <c r="C38" s="3">
-        <v>0.17599999999999999</v>
-      </c>
-      <c r="D38" s="17"/>
-      <c r="E38" s="5"/>
-      <c r="F38" s="17"/>
-    </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B39" s="14"/>
-      <c r="C39" s="3">
-        <v>0.17599999999999999</v>
-      </c>
-      <c r="D39" s="17"/>
-      <c r="E39" s="5"/>
-      <c r="F39" s="17"/>
-    </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B40" s="14"/>
-      <c r="C40" s="9">
-        <v>0.17299999999999999</v>
-      </c>
-      <c r="D40" s="17"/>
-      <c r="E40" s="5"/>
-      <c r="F40" s="17"/>
-    </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B41" s="14"/>
-      <c r="C41" s="12">
-        <v>0.17299999999999999</v>
-      </c>
-      <c r="D41" s="19"/>
-      <c r="E41" s="5"/>
-      <c r="F41" s="17"/>
-    </row>
-    <row r="42" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="15"/>
-      <c r="C42" s="11">
-        <v>0.182</v>
-      </c>
-      <c r="D42" s="18"/>
-      <c r="E42" s="6"/>
-      <c r="F42" s="18"/>
+      <c r="D43" s="15">
+        <f>AVERAGE(C43:C52)</f>
+        <v>0.18209999999999998</v>
+      </c>
+      <c r="F43" s="29">
+        <v>2047968</v>
+      </c>
+    </row>
+    <row r="44" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B44" s="31"/>
+      <c r="C44" s="30">
+        <v>0.17100000000000001</v>
+      </c>
+      <c r="D44" s="16"/>
+      <c r="F44" s="31"/>
+    </row>
+    <row r="45" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B45" s="31"/>
+      <c r="C45" s="30">
+        <v>0.17899999999999999</v>
+      </c>
+      <c r="D45" s="16"/>
+      <c r="F45" s="31"/>
+    </row>
+    <row r="46" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B46" s="31"/>
+      <c r="C46" s="30">
+        <v>0.184</v>
+      </c>
+      <c r="D46" s="16"/>
+      <c r="F46" s="31"/>
+    </row>
+    <row r="47" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B47" s="31"/>
+      <c r="C47" s="30">
+        <v>0.2</v>
+      </c>
+      <c r="D47" s="16"/>
+      <c r="F47" s="31"/>
+    </row>
+    <row r="48" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B48" s="31"/>
+      <c r="C48" s="30">
+        <v>0.189</v>
+      </c>
+      <c r="D48" s="16"/>
+      <c r="F48" s="31"/>
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B49" s="31"/>
+      <c r="C49" s="30">
+        <v>0.188</v>
+      </c>
+      <c r="D49" s="16"/>
+      <c r="F49" s="31"/>
+    </row>
+    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B50" s="31"/>
+      <c r="C50" s="30">
+        <v>0.17899999999999999</v>
+      </c>
+      <c r="D50" s="16"/>
+      <c r="F50" s="31"/>
+    </row>
+    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B51" s="31"/>
+      <c r="C51" s="30">
+        <v>0.17799999999999999</v>
+      </c>
+      <c r="D51" s="28"/>
+      <c r="F51" s="31"/>
+    </row>
+    <row r="52" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B52" s="31"/>
+      <c r="C52" s="30">
+        <v>0.17899999999999999</v>
+      </c>
+      <c r="D52" s="17"/>
+      <c r="F52" s="31"/>
+    </row>
+    <row r="53" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B53" s="31"/>
+      <c r="C53" s="30"/>
+      <c r="D53" s="15"/>
+    </row>
+    <row r="54" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B54" s="31"/>
+      <c r="C54" s="30"/>
+      <c r="D54" s="16"/>
+    </row>
+    <row r="55" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B55" s="31"/>
+      <c r="C55" s="30"/>
+      <c r="D55" s="16"/>
+    </row>
+    <row r="56" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B56" s="31"/>
+      <c r="C56" s="30"/>
+      <c r="D56" s="16"/>
+    </row>
+    <row r="57" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B57" s="31"/>
+      <c r="C57" s="30"/>
+      <c r="D57" s="16"/>
+    </row>
+    <row r="58" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B58" s="31"/>
+      <c r="C58" s="30"/>
+      <c r="D58" s="16"/>
+    </row>
+    <row r="59" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B59" s="31"/>
+      <c r="C59" s="30"/>
+      <c r="D59" s="16"/>
+    </row>
+    <row r="60" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B60" s="31"/>
+      <c r="C60" s="30"/>
+      <c r="D60" s="16"/>
+    </row>
+    <row r="61" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B61" s="31"/>
+      <c r="C61" s="30"/>
+      <c r="D61" s="28"/>
+    </row>
+    <row r="62" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B62" s="31"/>
+      <c r="C62" s="30"/>
+      <c r="D62" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="19">
+    <mergeCell ref="B43:B52"/>
+    <mergeCell ref="D43:D52"/>
+    <mergeCell ref="B53:B62"/>
+    <mergeCell ref="D53:D62"/>
+    <mergeCell ref="F43:F52"/>
+    <mergeCell ref="B23:B32"/>
+    <mergeCell ref="D23:D32"/>
+    <mergeCell ref="F23:F32"/>
+    <mergeCell ref="B33:B42"/>
+    <mergeCell ref="D33:D42"/>
+    <mergeCell ref="F33:F42"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="F3:F12"/>
     <mergeCell ref="F13:F22"/>
@@ -1204,13 +3414,8 @@
     <mergeCell ref="B13:B22"/>
     <mergeCell ref="D13:D22"/>
     <mergeCell ref="C2:D2"/>
-    <mergeCell ref="B23:B32"/>
-    <mergeCell ref="D23:D32"/>
-    <mergeCell ref="F23:F32"/>
-    <mergeCell ref="B33:B42"/>
-    <mergeCell ref="D33:D42"/>
-    <mergeCell ref="F33:F42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>